<commit_message>
v1 update NDC & NDC+ & LEP
</commit_message>
<xml_diff>
--- a/ssp_modeling/transformations/templates/calibrated/mexico/model_input_variables_mexico_se_calibrated.xlsx
+++ b/ssp_modeling/transformations/templates/calibrated/mexico/model_input_variables_mexico_se_calibrated.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
+    <sheet name="strategy_id-6002" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
   <si>
     <t>subsector</t>
   </si>
@@ -41,6 +42,114 @@
   </si>
   <si>
     <t>min_35</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
   </si>
   <si>
     <t>Economy</t>
@@ -471,121 +580,121 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>7</v>
-      </c>
-      <c r="R1" s="1">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="1">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="1">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="1">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="1">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="1">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AG1" s="1">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AH1" s="1">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AI1" s="1">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AJ1" s="1">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AK1" s="1">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AL1" s="1">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AM1" s="1">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AN1" s="1">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AO1" s="1">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AP1" s="1">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AQ1" s="1">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="1">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AS1" s="1">
+      <c r="AJ1" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:45">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -594,120 +703,120 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>1857.648102</v>
+        <v>2438.63</v>
       </c>
       <c r="K2">
-        <v>1869.8082082</v>
+        <v>2481.86</v>
       </c>
       <c r="L2">
-        <v>1881.9683144</v>
+        <v>2528.31</v>
       </c>
       <c r="M2">
-        <v>1894.1284206</v>
+        <v>2578.17</v>
       </c>
       <c r="N2">
-        <v>1906.2885268</v>
+        <v>2571</v>
       </c>
       <c r="O2">
-        <v>1918.448633</v>
+        <v>2348.57</v>
       </c>
       <c r="P2">
-        <v>1943.3463408</v>
+        <v>2485.67</v>
       </c>
       <c r="Q2">
-        <v>1968.2440486</v>
+        <v>2582.57</v>
       </c>
       <c r="R2">
-        <v>1993.1417564</v>
+        <v>2665.9611853</v>
       </c>
       <c r="S2">
-        <v>2018.0394642</v>
+        <v>2729.064486556051</v>
       </c>
       <c r="T2">
-        <v>2042.937172</v>
+        <v>2768.308433872728</v>
       </c>
       <c r="U2">
-        <v>2099.7419388</v>
+        <v>2821.875202068165</v>
       </c>
       <c r="V2">
-        <v>2156.5467056</v>
+        <v>2879.892956222686</v>
       </c>
       <c r="W2">
-        <v>2213.3514724</v>
+        <v>2939.247550050436</v>
       </c>
       <c r="X2">
-        <v>2270.1562392</v>
+        <v>2999.825442056975</v>
       </c>
       <c r="Y2">
-        <v>2326.961006</v>
+        <v>3064.774014262171</v>
       </c>
       <c r="Z2">
-        <v>2388.2460956</v>
+        <v>3133.687620037442</v>
       </c>
       <c r="AA2">
-        <v>2449.5311852</v>
+        <v>3206.767180385722</v>
       </c>
       <c r="AB2">
-        <v>2510.8162748</v>
+        <v>3284.228401143724</v>
       </c>
       <c r="AC2">
-        <v>2572.1013644</v>
+        <v>3366.302813475037</v>
       </c>
       <c r="AD2">
-        <v>2633.386454</v>
+        <v>3453.238902955263</v>
       </c>
       <c r="AE2">
-        <v>2698.6293606</v>
+        <v>3545.303334823448</v>
       </c>
       <c r="AF2">
-        <v>2763.8722672</v>
+        <v>3642.782283700117</v>
       </c>
       <c r="AG2">
-        <v>2829.1151738</v>
+        <v>3745.982876869395</v>
       </c>
       <c r="AH2">
-        <v>2894.3580804</v>
+        <v>3854.879962573155</v>
       </c>
       <c r="AI2">
-        <v>2959.600987</v>
+        <v>3969.092768170632</v>
       </c>
       <c r="AJ2">
-        <v>3030.6637982</v>
+        <v>4086.265089172769</v>
       </c>
       <c r="AK2">
-        <v>3101.7266094</v>
+        <v>4206.035987881747</v>
       </c>
       <c r="AL2">
-        <v>3172.7894206</v>
+        <v>4327.620495817171</v>
       </c>
       <c r="AM2">
-        <v>3243.8522318</v>
+        <v>4451.175014664492</v>
       </c>
       <c r="AN2">
-        <v>3314.915043</v>
+        <v>4576.865801935641</v>
       </c>
       <c r="AO2">
-        <v>3393.2952838</v>
+        <v>4704.294963972647</v>
       </c>
       <c r="AP2">
-        <v>3471.6755246</v>
+        <v>4833.390311373371</v>
       </c>
       <c r="AQ2">
-        <v>3550.0557654</v>
+        <v>4964.666776420458</v>
       </c>
       <c r="AR2">
-        <v>3628.4360062</v>
+        <v>5098.813058875173</v>
       </c>
       <c r="AS2">
-        <v>3706.816247</v>
+        <v>5236.227042493289</v>
       </c>
     </row>
     <row r="3" spans="1:45">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -826,10 +935,10 @@
     </row>
     <row r="4" spans="1:45">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -948,10 +1057,10 @@
     </row>
     <row r="5" spans="1:45">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1070,10 +1179,10 @@
     </row>
     <row r="6" spans="1:45">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="C6">
         <v>13</v>
@@ -1088,117 +1197,117 @@
         <v>1</v>
       </c>
       <c r="K6">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="N6">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="O6">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="P6">
-        <v>0.9399999999999999</v>
+        <v>1</v>
       </c>
       <c r="Q6">
-        <v>0.93</v>
+        <v>1</v>
       </c>
       <c r="R6">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="S6">
-        <v>0.91</v>
+        <v>1</v>
       </c>
       <c r="T6">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="U6">
-        <v>0.89</v>
+        <v>1</v>
       </c>
       <c r="V6">
-        <v>0.88</v>
+        <v>1</v>
       </c>
       <c r="W6">
-        <v>0.87</v>
+        <v>1</v>
       </c>
       <c r="X6">
-        <v>0.86</v>
+        <v>1</v>
       </c>
       <c r="Y6">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="Z6">
-        <v>0.84</v>
+        <v>1</v>
       </c>
       <c r="AA6">
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="AB6">
-        <v>0.82</v>
+        <v>1</v>
       </c>
       <c r="AC6">
-        <v>0.8100000000000001</v>
+        <v>1</v>
       </c>
       <c r="AD6">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AE6">
-        <v>0.79</v>
+        <v>1</v>
       </c>
       <c r="AF6">
-        <v>0.78</v>
+        <v>1</v>
       </c>
       <c r="AG6">
-        <v>0.77</v>
+        <v>1</v>
       </c>
       <c r="AH6">
-        <v>0.76</v>
+        <v>1</v>
       </c>
       <c r="AI6">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AJ6">
-        <v>0.74</v>
+        <v>1</v>
       </c>
       <c r="AK6">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="AL6">
-        <v>0.72</v>
+        <v>1</v>
       </c>
       <c r="AM6">
-        <v>0.71</v>
+        <v>1</v>
       </c>
       <c r="AN6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AO6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AP6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AQ6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AR6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AS6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:45">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -1317,10 +1426,10 @@
     </row>
     <row r="8" spans="1:45">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1439,10 +1548,10 @@
     </row>
     <row r="9" spans="1:45">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1561,10 +1670,10 @@
     </row>
     <row r="10" spans="1:45">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -1573,120 +1682,120 @@
         <v>1</v>
       </c>
       <c r="J10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="K10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="L10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="M10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="N10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="O10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="P10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="Q10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="R10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="S10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="T10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="U10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="V10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="W10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="X10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="Y10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="Z10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AA10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AB10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AC10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AD10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AE10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AF10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AG10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AH10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AI10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AJ10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AK10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AL10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AM10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AN10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AO10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AP10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AQ10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AR10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
       <c r="AS10">
-        <v>3.981666666666667</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="11" spans="1:45">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -1695,234 +1804,509 @@
         <v>1</v>
       </c>
       <c r="J11">
-        <v>25242936.69465</v>
+        <v>1270673.58425</v>
       </c>
       <c r="K11">
-        <v>25188375.99317</v>
+        <v>1281946.4346</v>
       </c>
       <c r="L11">
-        <v>25121419.04358</v>
+        <v>1293261.57585</v>
       </c>
       <c r="M11">
-        <v>25041298.78008</v>
+        <v>1304619.008</v>
       </c>
       <c r="N11">
-        <v>24948670.45124</v>
+        <v>1330724.4091</v>
       </c>
       <c r="O11">
-        <v>24844052.17557</v>
+        <v>1348317.33</v>
       </c>
       <c r="P11">
-        <v>24148167.4605303</v>
+        <v>1328499.46483333</v>
       </c>
       <c r="Q11">
-        <v>23982180.0528006</v>
+        <v>1308206.67733333</v>
       </c>
       <c r="R11">
-        <v>23816192.6450709</v>
+        <v>1287425.5225</v>
       </c>
       <c r="S11">
-        <v>23650205.2373412</v>
+        <v>1266144.704</v>
       </c>
       <c r="T11">
-        <v>23484217.8296115</v>
+        <v>1244362.12916667</v>
       </c>
       <c r="U11">
-        <v>23262838.7264268</v>
+        <v>1222095.888</v>
       </c>
       <c r="V11">
-        <v>23041459.6232421</v>
+        <v>1199322.599</v>
       </c>
       <c r="W11">
-        <v>22820080.5200574</v>
+        <v>1176036.76166667</v>
       </c>
       <c r="X11">
-        <v>22598701.4168727</v>
+        <v>1152236.1915</v>
       </c>
       <c r="Y11">
-        <v>22377322.313688</v>
+        <v>1127922.22</v>
       </c>
       <c r="Z11">
-        <v>22104162.687993</v>
+        <v>1103099.38633333</v>
       </c>
       <c r="AA11">
-        <v>21831003.062298</v>
+        <v>1077775.762</v>
       </c>
       <c r="AB11">
-        <v>21557843.436603</v>
+        <v>1051962.95966667</v>
       </c>
       <c r="AC11">
-        <v>21284683.810908</v>
+        <v>1025675.07466667</v>
       </c>
       <c r="AD11">
-        <v>21011524.185213</v>
+        <v>998926.775</v>
       </c>
       <c r="AE11">
-        <v>20693436.1423304</v>
+        <v>971734.296</v>
       </c>
       <c r="AF11">
-        <v>20375348.0994478</v>
+        <v>944114.411333333</v>
       </c>
       <c r="AG11">
-        <v>20057260.0565652</v>
+        <v>916083.03</v>
       </c>
       <c r="AH11">
-        <v>19739172.0136826</v>
+        <v>887656.569833333</v>
       </c>
       <c r="AI11">
-        <v>19421083.9708</v>
+        <v>858850.933333333</v>
       </c>
       <c r="AJ11">
-        <v>19064337.7234435</v>
+        <v>829681.9125</v>
       </c>
       <c r="AK11">
-        <v>18707591.476087</v>
+        <v>800165.333333333</v>
       </c>
       <c r="AL11">
-        <v>18350845.2287305</v>
+        <v>770315.981</v>
       </c>
       <c r="AM11">
-        <v>17994098.981374</v>
+        <v>740149.213</v>
       </c>
       <c r="AN11">
-        <v>17637352.7340175</v>
+        <v>709679.380833333</v>
       </c>
       <c r="AO11">
-        <v>17249043.5632184</v>
+        <v>678919.5820000001</v>
       </c>
       <c r="AP11">
-        <v>16860734.3924193</v>
+        <v>647877.7755</v>
       </c>
       <c r="AQ11">
-        <v>16472425.2216202</v>
+        <v>616562.955666666</v>
       </c>
       <c r="AR11">
-        <v>16084116.0508211</v>
+        <v>584982.686166666</v>
       </c>
       <c r="AS11">
-        <v>15695806.880022</v>
+        <v>553142.3</v>
       </c>
     </row>
     <row r="12" spans="1:45">
       <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>3324890.91575</v>
+      </c>
+      <c r="K12">
+        <v>3326056.5654</v>
+      </c>
+      <c r="L12">
+        <v>3327179.92415</v>
+      </c>
+      <c r="M12">
+        <v>3328260.992</v>
+      </c>
+      <c r="N12">
+        <v>3366502.5909</v>
+      </c>
+      <c r="O12">
+        <v>3382620.67</v>
+      </c>
+      <c r="P12">
+        <v>3435993.53516667</v>
+      </c>
+      <c r="Q12">
+        <v>3489617.32266667</v>
+      </c>
+      <c r="R12">
+        <v>3543439.4775</v>
+      </c>
+      <c r="S12">
+        <v>3597407.296</v>
+      </c>
+      <c r="T12">
+        <v>3651488.87083333</v>
+      </c>
+      <c r="U12">
+        <v>3705710.112</v>
+      </c>
+      <c r="V12">
+        <v>3759971.401</v>
+      </c>
+      <c r="W12">
+        <v>3814218.23833333</v>
+      </c>
+      <c r="X12">
+        <v>3868400.8085</v>
+      </c>
+      <c r="Y12">
+        <v>3922475.78</v>
+      </c>
+      <c r="Z12">
+        <v>3976406.61366667</v>
+      </c>
+      <c r="AA12">
+        <v>4030166.238</v>
+      </c>
+      <c r="AB12">
+        <v>4083739.04033333</v>
+      </c>
+      <c r="AC12">
+        <v>4137118.92533333</v>
+      </c>
+      <c r="AD12">
+        <v>4190303.225</v>
+      </c>
+      <c r="AE12">
+        <v>4243297.704</v>
+      </c>
+      <c r="AF12">
+        <v>4296113.58866667</v>
+      </c>
+      <c r="AG12">
+        <v>4348761.97</v>
+      </c>
+      <c r="AH12">
+        <v>4401260.43016667</v>
+      </c>
+      <c r="AI12">
+        <v>4453629.06666667</v>
+      </c>
+      <c r="AJ12">
+        <v>4505893.0875</v>
+      </c>
+      <c r="AK12">
+        <v>4558084.66666667</v>
+      </c>
+      <c r="AL12">
+        <v>4610238.019</v>
+      </c>
+      <c r="AM12">
+        <v>4662399.787</v>
+      </c>
+      <c r="AN12">
+        <v>4714621.61916667</v>
+      </c>
+      <c r="AO12">
+        <v>4766959.418</v>
+      </c>
+      <c r="AP12">
+        <v>4819445.2245</v>
+      </c>
+      <c r="AQ12">
+        <v>4872128.04433333</v>
+      </c>
+      <c r="AR12">
+        <v>4925058.31383333</v>
+      </c>
+      <c r="AS12">
+        <v>4978280.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>96615314.30535001</v>
-      </c>
-      <c r="K12">
-        <v>98145003.00683001</v>
-      </c>
-      <c r="L12">
-        <v>99655906.95642</v>
-      </c>
-      <c r="M12">
-        <v>101149483.21992</v>
-      </c>
-      <c r="N12">
-        <v>102626858.54876</v>
-      </c>
-      <c r="O12">
-        <v>104088700.82443</v>
-      </c>
-      <c r="P12">
-        <v>103160360.35947</v>
-      </c>
-      <c r="Q12">
-        <v>104452121.587199</v>
-      </c>
-      <c r="R12">
-        <v>105743882.814929</v>
-      </c>
-      <c r="S12">
-        <v>107035644.042659</v>
-      </c>
-      <c r="T12">
-        <v>108327405.270388</v>
-      </c>
-      <c r="U12">
-        <v>109535912.593573</v>
-      </c>
-      <c r="V12">
-        <v>110744419.916758</v>
-      </c>
-      <c r="W12">
-        <v>111952927.239943</v>
-      </c>
-      <c r="X12">
-        <v>113161434.563127</v>
-      </c>
-      <c r="Y12">
-        <v>114369941.886312</v>
-      </c>
-      <c r="Z12">
-        <v>115475285.912007</v>
-      </c>
-      <c r="AA12">
-        <v>116580629.937702</v>
-      </c>
-      <c r="AB12">
-        <v>117685973.963397</v>
-      </c>
-      <c r="AC12">
-        <v>118791317.989092</v>
-      </c>
-      <c r="AD12">
-        <v>119896662.014787</v>
-      </c>
-      <c r="AE12">
-        <v>120892736.81767</v>
-      </c>
-      <c r="AF12">
-        <v>121888811.620552</v>
-      </c>
-      <c r="AG12">
-        <v>122884886.423435</v>
-      </c>
-      <c r="AH12">
-        <v>123880961.226317</v>
-      </c>
-      <c r="AI12">
-        <v>124877036.0292</v>
-      </c>
-      <c r="AJ12">
-        <v>125753832.176556</v>
-      </c>
-      <c r="AK12">
-        <v>126630628.323913</v>
-      </c>
-      <c r="AL12">
-        <v>127507424.47127</v>
-      </c>
-      <c r="AM12">
-        <v>128384220.618626</v>
-      </c>
-      <c r="AN12">
-        <v>129261016.765983</v>
-      </c>
-      <c r="AO12">
-        <v>130013458.896782</v>
-      </c>
-      <c r="AP12">
-        <v>130765901.027581</v>
-      </c>
-      <c r="AQ12">
-        <v>131518343.15838</v>
-      </c>
-      <c r="AR12">
-        <v>132270785.289179</v>
-      </c>
-      <c r="AS12">
-        <v>133023227.419978</v>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>0.9782608695652174</v>
+      </c>
+      <c r="X2">
+        <v>0.9565217391304348</v>
+      </c>
+      <c r="Y2">
+        <v>0.9347826086956521</v>
+      </c>
+      <c r="Z2">
+        <v>0.9130434782608696</v>
+      </c>
+      <c r="AA2">
+        <v>0.891304347826087</v>
+      </c>
+      <c r="AB2">
+        <v>0.8695652173913043</v>
+      </c>
+      <c r="AC2">
+        <v>0.8478260869565217</v>
+      </c>
+      <c r="AD2">
+        <v>0.8260869565217391</v>
+      </c>
+      <c r="AE2">
+        <v>0.8043478260869565</v>
+      </c>
+      <c r="AF2">
+        <v>0.7826086956521739</v>
+      </c>
+      <c r="AG2">
+        <v>0.7608695652173914</v>
+      </c>
+      <c r="AH2">
+        <v>0.7391304347826086</v>
+      </c>
+      <c r="AI2">
+        <v>0.7173913043478262</v>
+      </c>
+      <c r="AJ2">
+        <v>0.6956521739130435</v>
+      </c>
+      <c r="AK2">
+        <v>0.6739130434782609</v>
+      </c>
+      <c r="AL2">
+        <v>0.6521739130434783</v>
+      </c>
+      <c r="AM2">
+        <v>0.6304347826086957</v>
+      </c>
+      <c r="AN2">
+        <v>0.6086956521739131</v>
+      </c>
+      <c r="AO2">
+        <v>0.5869565217391304</v>
+      </c>
+      <c r="AP2">
+        <v>0.5652173913043479</v>
+      </c>
+      <c r="AQ2">
+        <v>0.5434782608695652</v>
+      </c>
+      <c r="AR2">
+        <v>0.5217391304347826</v>
+      </c>
+      <c r="AS2">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>